<commit_message>
added blue rockfish habitat level 3
</commit_message>
<xml_diff>
--- a/Data/RAMassessmentreviewsSept13_2017.xlsx
+++ b/Data/RAMassessmentreviewsSept13_2017.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kristin.marshall/Rprojects/EcoStockAssess/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{82C77EA6-87E3-9A4F-BB15-0BDC93357BF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10380" yWindow="-26560" windowWidth="37860" windowHeight="25320" tabRatio="500"/>
+    <workbookView xWindow="6440" yWindow="-25320" windowWidth="37860" windowHeight="25320" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scores_Sept13_output_to_CSV" sheetId="5" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">AssessmentScores_RAW_w_Comments!$A$1:$AL$234</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Scores_Sept13_output_to_CSV!$A$1:$V$207</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -34,13 +35,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
     <author>Kristin Marshall</author>
   </authors>
   <commentList>
-    <comment ref="H1" authorId="0">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -57,7 +58,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="H2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -69,7 +70,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M5" authorId="0">
+    <comment ref="M5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -94,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K7" authorId="0">
+    <comment ref="K7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -106,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0">
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -119,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L12" authorId="0">
+    <comment ref="L12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H15" authorId="0">
+    <comment ref="H15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000008000000}">
       <text>
         <r>
           <rPr>
@@ -143,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L15" authorId="0">
+    <comment ref="L15" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000009000000}">
       <text>
         <r>
           <rPr>
@@ -155,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M21" authorId="0">
+    <comment ref="M21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -167,7 +168,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H23" authorId="0">
+    <comment ref="H23" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -179,7 +180,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H25" authorId="0">
+    <comment ref="H25" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -191,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H26" authorId="0">
+    <comment ref="H26" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -203,7 +204,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L28" authorId="0">
+    <comment ref="L28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -215,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M28" authorId="0">
+    <comment ref="M28" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -228,7 +229,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L30" authorId="0">
+    <comment ref="L30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000010000000}">
       <text>
         <r>
           <rPr>
@@ -240,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M30" authorId="0">
+    <comment ref="M30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000011000000}">
       <text>
         <r>
           <rPr>
@@ -253,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M31" authorId="0">
+    <comment ref="M31" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000012000000}">
       <text>
         <r>
           <rPr>
@@ -265,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H32" authorId="0">
+    <comment ref="H32" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000013000000}">
       <text>
         <r>
           <rPr>
@@ -277,7 +278,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L35" authorId="0">
+    <comment ref="L35" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000014000000}">
       <text>
         <r>
           <rPr>
@@ -290,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H37" authorId="1">
+    <comment ref="H37" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000015000000}">
       <text>
         <r>
           <rPr>
@@ -314,7 +315,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L38" authorId="0">
+    <comment ref="L38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000016000000}">
       <text>
         <r>
           <rPr>
@@ -327,7 +328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L39" authorId="1">
+    <comment ref="L39" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000017000000}">
       <text>
         <r>
           <rPr>
@@ -351,7 +352,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M41" authorId="0">
+    <comment ref="M41" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000018000000}">
       <text>
         <r>
           <rPr>
@@ -364,7 +365,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M42" authorId="0">
+    <comment ref="M42" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000019000000}">
       <text>
         <r>
           <rPr>
@@ -377,7 +378,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M43" authorId="0">
+    <comment ref="M43" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -390,7 +391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L44" authorId="0">
+    <comment ref="L44" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -402,7 +403,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H55" authorId="1">
+    <comment ref="H55" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -426,7 +427,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L57" authorId="0">
+    <comment ref="L57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -438,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M57" authorId="0">
+    <comment ref="M57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -450,7 +451,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L58" authorId="1">
+    <comment ref="L58" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -474,7 +475,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H59" authorId="1">
+    <comment ref="H59" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000020000000}">
       <text>
         <r>
           <rPr>
@@ -498,7 +499,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D62" authorId="1">
+    <comment ref="D62" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000021000000}">
       <text>
         <r>
           <rPr>
@@ -522,7 +523,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L62" authorId="0">
+    <comment ref="L62" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000022000000}">
       <text>
         <r>
           <rPr>
@@ -534,7 +535,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L65" authorId="1">
+    <comment ref="L65" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000023000000}">
       <text>
         <r>
           <rPr>
@@ -558,7 +559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L66" authorId="0">
+    <comment ref="L66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000024000000}">
       <text>
         <r>
           <rPr>
@@ -571,7 +572,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M66" authorId="0">
+    <comment ref="M66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000025000000}">
       <text>
         <r>
           <rPr>
@@ -584,7 +585,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D69" authorId="0">
+    <comment ref="D69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000026000000}">
       <text>
         <r>
           <rPr>
@@ -596,7 +597,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H76" authorId="0">
+    <comment ref="H76" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000027000000}">
       <text>
         <r>
           <rPr>
@@ -608,7 +609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H77" authorId="0">
+    <comment ref="H77" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000028000000}">
       <text>
         <r>
           <rPr>
@@ -621,7 +622,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L77" authorId="0">
+    <comment ref="L77" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000029000000}">
       <text>
         <r>
           <rPr>
@@ -634,7 +635,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L79" authorId="0">
+    <comment ref="L79" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -646,7 +647,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M80" authorId="0">
+    <comment ref="M80" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -659,7 +660,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K81" authorId="0">
+    <comment ref="K81" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -672,7 +673,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L81" authorId="0">
+    <comment ref="L81" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -685,7 +686,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M81" authorId="0">
+    <comment ref="M81" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -698,7 +699,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M82" authorId="0">
+    <comment ref="M82" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -711,7 +712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M83" authorId="0">
+    <comment ref="M83" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000030000000}">
       <text>
         <r>
           <rPr>
@@ -724,7 +725,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M84" authorId="0">
+    <comment ref="M84" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000031000000}">
       <text>
         <r>
           <rPr>
@@ -737,7 +738,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M85" authorId="0">
+    <comment ref="M85" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000032000000}">
       <text>
         <r>
           <rPr>
@@ -750,7 +751,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M86" authorId="0">
+    <comment ref="M86" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000033000000}">
       <text>
         <r>
           <rPr>
@@ -763,7 +764,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M87" authorId="0">
+    <comment ref="M87" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000034000000}">
       <text>
         <r>
           <rPr>
@@ -776,7 +777,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M88" authorId="0">
+    <comment ref="M88" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000035000000}">
       <text>
         <r>
           <rPr>
@@ -789,7 +790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M89" authorId="0">
+    <comment ref="M89" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000036000000}">
       <text>
         <r>
           <rPr>
@@ -802,7 +803,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M90" authorId="0">
+    <comment ref="M90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000037000000}">
       <text>
         <r>
           <rPr>
@@ -815,7 +816,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M91" authorId="0">
+    <comment ref="M91" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000038000000}">
       <text>
         <r>
           <rPr>
@@ -828,7 +829,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M92" authorId="0">
+    <comment ref="M92" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000039000000}">
       <text>
         <r>
           <rPr>
@@ -841,7 +842,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K98" authorId="0">
+    <comment ref="K98" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003A000000}">
       <text>
         <r>
           <rPr>
@@ -853,7 +854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L98" authorId="0">
+    <comment ref="L98" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003B000000}">
       <text>
         <r>
           <rPr>
@@ -865,7 +866,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L99" authorId="0">
+    <comment ref="L99" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003C000000}">
       <text>
         <r>
           <rPr>
@@ -877,7 +878,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K100" authorId="1">
+    <comment ref="K100" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003D000000}">
       <text>
         <r>
           <rPr>
@@ -902,7 +903,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L100" authorId="1">
+    <comment ref="L100" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003E000000}">
       <text>
         <r>
           <rPr>
@@ -926,7 +927,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L102" authorId="0">
+    <comment ref="L102" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00003F000000}">
       <text>
         <r>
           <rPr>
@@ -939,7 +940,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L106" authorId="0">
+    <comment ref="L106" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000040000000}">
       <text>
         <r>
           <rPr>
@@ -951,7 +952,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H108" authorId="0">
+    <comment ref="H108" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000041000000}">
       <text>
         <r>
           <rPr>
@@ -964,7 +965,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L108" authorId="0">
+    <comment ref="L108" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000042000000}">
       <text>
         <r>
           <rPr>
@@ -977,7 +978,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H114" authorId="1">
+    <comment ref="H114" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000043000000}">
       <text>
         <r>
           <rPr>
@@ -1001,7 +1002,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L114" authorId="1">
+    <comment ref="L114" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000044000000}">
       <text>
         <r>
           <rPr>
@@ -1025,7 +1026,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L119" authorId="1">
+    <comment ref="L119" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000045000000}">
       <text>
         <r>
           <rPr>
@@ -1049,7 +1050,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H120" authorId="1">
+    <comment ref="H120" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000046000000}">
       <text>
         <r>
           <rPr>
@@ -1073,7 +1074,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L146" authorId="0">
+    <comment ref="L146" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000047000000}">
       <text>
         <r>
           <rPr>
@@ -1086,7 +1087,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H150" authorId="1">
+    <comment ref="H150" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000048000000}">
       <text>
         <r>
           <rPr>
@@ -1110,7 +1111,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H151" authorId="0">
+    <comment ref="H151" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000049000000}">
       <text>
         <r>
           <rPr>
@@ -1123,7 +1124,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K151" authorId="0">
+    <comment ref="K151" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004A000000}">
       <text>
         <r>
           <rPr>
@@ -1136,7 +1137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H153" authorId="1">
+    <comment ref="H153" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004B000000}">
       <text>
         <r>
           <rPr>
@@ -1160,7 +1161,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L153" authorId="1">
+    <comment ref="L153" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004C000000}">
       <text>
         <r>
           <rPr>
@@ -1184,7 +1185,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L154" authorId="1">
+    <comment ref="L154" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004D000000}">
       <text>
         <r>
           <rPr>
@@ -1208,7 +1209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H155" authorId="0">
+    <comment ref="H155" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004E000000}">
       <text>
         <r>
           <rPr>
@@ -1221,7 +1222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I155" authorId="0">
+    <comment ref="I155" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00004F000000}">
       <text>
         <r>
           <rPr>
@@ -1234,7 +1235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H157" authorId="1">
+    <comment ref="H157" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000050000000}">
       <text>
         <r>
           <rPr>
@@ -1258,7 +1259,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L158" authorId="1">
+    <comment ref="L158" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0000-000051000000}">
       <text>
         <r>
           <rPr>
@@ -1282,7 +1283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I159" authorId="0">
+    <comment ref="I159" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000052000000}">
       <text>
         <r>
           <rPr>
@@ -1294,7 +1295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L165" authorId="0">
+    <comment ref="L165" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000053000000}">
       <text>
         <r>
           <rPr>
@@ -1306,7 +1307,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L166" authorId="0">
+    <comment ref="L166" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000054000000}">
       <text>
         <r>
           <rPr>
@@ -1319,7 +1320,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H172" authorId="0">
+    <comment ref="H172" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000055000000}">
       <text>
         <r>
           <rPr>
@@ -1331,7 +1332,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J172" authorId="0">
+    <comment ref="J172" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000056000000}">
       <text>
         <r>
           <rPr>
@@ -1343,7 +1344,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K172" authorId="0">
+    <comment ref="K172" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000057000000}">
       <text>
         <r>
           <rPr>
@@ -1355,7 +1356,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L174" authorId="0">
+    <comment ref="L174" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000058000000}">
       <text>
         <r>
           <rPr>
@@ -1370,7 +1371,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M174" authorId="0">
+    <comment ref="M174" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000059000000}">
       <text>
         <r>
           <rPr>
@@ -1383,7 +1384,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L181" authorId="0">
+    <comment ref="L181" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005A000000}">
       <text>
         <r>
           <rPr>
@@ -1397,7 +1398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K182" authorId="0">
+    <comment ref="K182" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005B000000}">
       <text>
         <r>
           <rPr>
@@ -1410,7 +1411,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L184" authorId="0">
+    <comment ref="L184" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005C000000}">
       <text>
         <r>
           <rPr>
@@ -1423,7 +1424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M185" authorId="0">
+    <comment ref="M185" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005D000000}">
       <text>
         <r>
           <rPr>
@@ -1436,7 +1437,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L186" authorId="0">
+    <comment ref="L186" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005E000000}">
       <text>
         <r>
           <rPr>
@@ -1449,7 +1450,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M186" authorId="0">
+    <comment ref="M186" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00005F000000}">
       <text>
         <r>
           <rPr>
@@ -1462,7 +1463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A188" authorId="0">
+    <comment ref="A188" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000060000000}">
       <text>
         <r>
           <rPr>
@@ -1475,7 +1476,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M190" authorId="0">
+    <comment ref="M190" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000061000000}">
       <text>
         <r>
           <rPr>
@@ -1488,7 +1489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N190" authorId="0">
+    <comment ref="N190" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000062000000}">
       <text>
         <r>
           <rPr>
@@ -1501,7 +1502,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H191" authorId="0">
+    <comment ref="H191" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000063000000}">
       <text>
         <r>
           <rPr>
@@ -1514,7 +1515,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J192" authorId="0">
+    <comment ref="J192" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000064000000}">
       <text>
         <r>
           <rPr>
@@ -1527,7 +1528,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M192" authorId="0">
+    <comment ref="M192" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000065000000}">
       <text>
         <r>
           <rPr>
@@ -1540,7 +1541,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K194" authorId="0">
+    <comment ref="K194" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000066000000}">
       <text>
         <r>
           <rPr>
@@ -1553,7 +1554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A196" authorId="0">
+    <comment ref="A196" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000067000000}">
       <text>
         <r>
           <rPr>
@@ -1566,7 +1567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L197" authorId="0">
+    <comment ref="L197" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000068000000}">
       <text>
         <r>
           <rPr>
@@ -1579,7 +1580,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N197" authorId="0">
+    <comment ref="N197" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000069000000}">
       <text>
         <r>
           <rPr>
@@ -1592,7 +1593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H198" authorId="0">
+    <comment ref="H198" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006A000000}">
       <text>
         <r>
           <rPr>
@@ -1605,7 +1606,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L199" authorId="0">
+    <comment ref="L199" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006B000000}">
       <text>
         <r>
           <rPr>
@@ -1618,7 +1619,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J200" authorId="0">
+    <comment ref="J200" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006C000000}">
       <text>
         <r>
           <rPr>
@@ -1631,7 +1632,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L200" authorId="0">
+    <comment ref="L200" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006D000000}">
       <text>
         <r>
           <rPr>
@@ -1644,7 +1645,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M200" authorId="0">
+    <comment ref="M200" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006E000000}">
       <text>
         <r>
           <rPr>
@@ -1657,7 +1658,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J201" authorId="0">
+    <comment ref="J201" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-00006F000000}">
       <text>
         <r>
           <rPr>
@@ -1670,7 +1671,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M201" authorId="0">
+    <comment ref="M201" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000070000000}">
       <text>
         <r>
           <rPr>
@@ -1683,7 +1684,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M202" authorId="0">
+    <comment ref="M202" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000071000000}">
       <text>
         <r>
           <rPr>
@@ -1696,7 +1697,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A203" authorId="0">
+    <comment ref="A203" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000072000000}">
       <text>
         <r>
           <rPr>
@@ -1709,7 +1710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K205" authorId="0">
+    <comment ref="K205" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000073000000}">
       <text>
         <r>
           <rPr>
@@ -1722,7 +1723,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K206" authorId="0">
+    <comment ref="K206" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000074000000}">
       <text>
         <r>
           <rPr>
@@ -1735,7 +1736,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M206" authorId="0">
+    <comment ref="M206" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000075000000}">
       <text>
         <r>
           <rPr>
@@ -1748,7 +1749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M207" authorId="0">
+    <comment ref="M207" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000076000000}">
       <text>
         <r>
           <rPr>
@@ -1761,7 +1762,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N207" authorId="0">
+    <comment ref="N207" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000077000000}">
       <text>
         <r>
           <rPr>
@@ -1779,13 +1780,14 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
     <author>Kristin Marshall</author>
+    <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -1793,16 +1795,56 @@
             <color rgb="FF000000"/>
             <rFont val="Arial"/>
           </rPr>
-          <t>Code for scoring:
-0= no mention anywhere
-1= mentioned as background information
-2= explicit consideration of effect of the factor on the fishery or fishery on the factor (e.g. estimates of predation mortality provided, but not used in assessment model)
-3= attempt to include in the assessment model (even if thrown out)
-	-Kristin Marshall</t>
+          <t xml:space="preserve">Code for scoring:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">0= no mention anywhere
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">1= mentioned as background information
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">2= explicit consideration of effect of the factor on the fishery or fishery on the factor (e.g. estimates of predation mortality provided, but not used in assessment model)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">3= attempt to include in the assessment model (even if thrown out)
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+          </rPr>
+          <t xml:space="preserve">	-Kristin Marshall</t>
         </r>
       </text>
     </comment>
-    <comment ref="M2" authorId="0">
+    <comment ref="M2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -1814,7 +1856,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N6" authorId="0">
+    <comment ref="N6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -1827,7 +1869,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O6" authorId="0">
+    <comment ref="O6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -1840,7 +1882,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="1">
+    <comment ref="F9" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -1864,7 +1906,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N9" authorId="0">
+    <comment ref="N9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -1876,7 +1918,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="1">
+    <comment ref="J11" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -1900,7 +1942,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N12" authorId="0">
+    <comment ref="N12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -1913,7 +1955,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J16" authorId="1">
+    <comment ref="J16" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000009000000}">
       <text>
         <r>
           <rPr>
@@ -1937,7 +1979,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M19" authorId="0">
+    <comment ref="M19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -1949,7 +1991,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N19" authorId="0">
+    <comment ref="N19" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -1962,7 +2004,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N20" authorId="0">
+    <comment ref="N20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -1975,7 +2017,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G22" authorId="0">
+    <comment ref="G22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000D000000}">
       <text>
         <r>
           <rPr>
@@ -1988,7 +2030,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N22" authorId="0">
+    <comment ref="N22" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000E000000}">
       <text>
         <r>
           <rPr>
@@ -2001,7 +2043,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J27" authorId="1">
+    <comment ref="J27" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-00000F000000}">
       <text>
         <r>
           <rPr>
@@ -2025,7 +2067,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N27" authorId="1">
+    <comment ref="N27" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000010000000}">
       <text>
         <r>
           <rPr>
@@ -2049,7 +2091,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J29" authorId="0">
+    <comment ref="J29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000011000000}">
       <text>
         <r>
           <rPr>
@@ -2062,7 +2104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N29" authorId="0">
+    <comment ref="N29" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000012000000}">
       <text>
         <r>
           <rPr>
@@ -2075,7 +2117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J30" authorId="0">
+    <comment ref="J30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000013000000}">
       <text>
         <r>
           <rPr>
@@ -2088,7 +2130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M30" authorId="0">
+    <comment ref="M30" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000014000000}">
       <text>
         <r>
           <rPr>
@@ -2101,7 +2143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J33" authorId="1">
+    <comment ref="J33" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000015000000}">
       <text>
         <r>
           <rPr>
@@ -2125,7 +2167,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M42" authorId="1">
+    <comment ref="M42" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000016000000}">
       <text>
         <r>
           <rPr>
@@ -2150,7 +2192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N42" authorId="1">
+    <comment ref="N42" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000017000000}">
       <text>
         <r>
           <rPr>
@@ -2174,7 +2216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N44" authorId="0">
+    <comment ref="N44" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000018000000}">
       <text>
         <r>
           <rPr>
@@ -2186,7 +2228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J45" authorId="0">
+    <comment ref="J45" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000019000000}">
       <text>
         <r>
           <rPr>
@@ -2199,7 +2241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M45" authorId="0">
+    <comment ref="M45" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001A000000}">
       <text>
         <r>
           <rPr>
@@ -2212,7 +2254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O45" authorId="0">
+    <comment ref="O45" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001B000000}">
       <text>
         <r>
           <rPr>
@@ -2225,7 +2267,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N48" authorId="0">
+    <comment ref="N48" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001C000000}">
       <text>
         <r>
           <rPr>
@@ -2237,7 +2279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N50" authorId="0">
+    <comment ref="N50" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001D000000}">
       <text>
         <r>
           <rPr>
@@ -2250,7 +2292,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J52" authorId="0">
+    <comment ref="J52" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001E000000}">
       <text>
         <r>
           <rPr>
@@ -2262,7 +2304,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L52" authorId="0">
+    <comment ref="L52" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00001F000000}">
       <text>
         <r>
           <rPr>
@@ -2274,7 +2316,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M52" authorId="0">
+    <comment ref="M52" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000020000000}">
       <text>
         <r>
           <rPr>
@@ -2286,7 +2328,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N57" authorId="0">
+    <comment ref="N57" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000021000000}">
       <text>
         <r>
           <rPr>
@@ -2298,7 +2340,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N59" authorId="0">
+    <comment ref="N59" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000022000000}">
       <text>
         <r>
           <rPr>
@@ -2311,7 +2353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N63" authorId="0">
+    <comment ref="N63" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000023000000}">
       <text>
         <r>
           <rPr>
@@ -2324,7 +2366,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N67" authorId="0">
+    <comment ref="N67" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000024000000}">
       <text>
         <r>
           <rPr>
@@ -2337,7 +2379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O67" authorId="0">
+    <comment ref="O67" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000025000000}">
       <text>
         <r>
           <rPr>
@@ -2350,7 +2392,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N68" authorId="0">
+    <comment ref="N68" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000026000000}">
       <text>
         <r>
           <rPr>
@@ -2362,7 +2404,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O68" authorId="0">
+    <comment ref="O68" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000027000000}">
       <text>
         <r>
           <rPr>
@@ -2375,7 +2417,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N69" authorId="0">
+    <comment ref="N69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000028000000}">
       <text>
         <r>
           <rPr>
@@ -2387,7 +2429,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O69" authorId="0">
+    <comment ref="O69" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000029000000}">
       <text>
         <r>
           <rPr>
@@ -2400,7 +2442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J73" authorId="0">
+    <comment ref="J73" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002A000000}">
       <text>
         <r>
           <rPr>
@@ -2413,7 +2455,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N75" authorId="0">
+    <comment ref="N75" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002B000000}">
       <text>
         <r>
           <rPr>
@@ -2426,7 +2468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J79" authorId="0">
+    <comment ref="J79" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002C000000}">
       <text>
         <r>
           <rPr>
@@ -2439,7 +2481,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M82" authorId="0">
+    <comment ref="M82" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002D000000}">
       <text>
         <r>
           <rPr>
@@ -2451,7 +2493,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N82" authorId="0">
+    <comment ref="N82" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002E000000}">
       <text>
         <r>
           <rPr>
@@ -2463,7 +2505,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N84" authorId="0">
+    <comment ref="N84" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00002F000000}">
       <text>
         <r>
           <rPr>
@@ -2477,7 +2519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L85" authorId="0">
+    <comment ref="L85" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000030000000}">
       <text>
         <r>
           <rPr>
@@ -2490,7 +2532,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N85" authorId="0">
+    <comment ref="N85" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000031000000}">
       <text>
         <r>
           <rPr>
@@ -2503,7 +2545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O85" authorId="0">
+    <comment ref="O85" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000032000000}">
       <text>
         <r>
           <rPr>
@@ -2516,7 +2558,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J86" authorId="0">
+    <comment ref="J86" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000033000000}">
       <text>
         <r>
           <rPr>
@@ -2529,7 +2571,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K86" authorId="0">
+    <comment ref="K86" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000034000000}">
       <text>
         <r>
           <rPr>
@@ -2542,7 +2584,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L87" authorId="0">
+    <comment ref="L87" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000035000000}">
       <text>
         <r>
           <rPr>
@@ -2555,7 +2597,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O87" authorId="0">
+    <comment ref="O87" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000036000000}">
       <text>
         <r>
           <rPr>
@@ -2568,7 +2610,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A89" authorId="0">
+    <comment ref="A89" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000037000000}">
       <text>
         <r>
           <rPr>
@@ -2581,7 +2623,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M90" authorId="0">
+    <comment ref="M90" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000038000000}">
       <text>
         <r>
           <rPr>
@@ -2594,7 +2636,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O92" authorId="0">
+    <comment ref="O92" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000039000000}">
       <text>
         <r>
           <rPr>
@@ -2607,7 +2649,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L95" authorId="0">
+    <comment ref="L95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003A000000}">
       <text>
         <r>
           <rPr>
@@ -2620,7 +2662,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O95" authorId="0">
+    <comment ref="O95" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003B000000}">
       <text>
         <r>
           <rPr>
@@ -2633,7 +2675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O96" authorId="0">
+    <comment ref="O96" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003C000000}">
       <text>
         <r>
           <rPr>
@@ -2646,7 +2688,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J99" authorId="1">
+    <comment ref="J99" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003D000000}">
       <text>
         <r>
           <rPr>
@@ -2670,7 +2712,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N99" authorId="1">
+    <comment ref="N99" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003E000000}">
       <text>
         <r>
           <rPr>
@@ -2694,7 +2736,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M100" authorId="0">
+    <comment ref="M100" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00003F000000}">
       <text>
         <r>
           <rPr>
@@ -2707,7 +2749,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N103" authorId="0">
+    <comment ref="N103" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000040000000}">
       <text>
         <r>
           <rPr>
@@ -2722,7 +2764,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O103" authorId="0">
+    <comment ref="O103" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000041000000}">
       <text>
         <r>
           <rPr>
@@ -2735,7 +2777,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A105" authorId="0">
+    <comment ref="A105" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000042000000}">
       <text>
         <r>
           <rPr>
@@ -2748,7 +2790,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A106" authorId="0">
+    <comment ref="A106" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000043000000}">
       <text>
         <r>
           <rPr>
@@ -2761,7 +2803,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N107" authorId="0">
+    <comment ref="N107" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000044000000}">
       <text>
         <r>
           <rPr>
@@ -2774,7 +2816,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P107" authorId="0">
+    <comment ref="P107" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000045000000}">
       <text>
         <r>
           <rPr>
@@ -2787,7 +2829,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N108" authorId="0">
+    <comment ref="N108" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000046000000}">
       <text>
         <r>
           <rPr>
@@ -2800,7 +2842,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O108" authorId="0">
+    <comment ref="O108" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000047000000}">
       <text>
         <r>
           <rPr>
@@ -2813,7 +2855,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N109" authorId="0">
+    <comment ref="N109" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000048000000}">
       <text>
         <r>
           <rPr>
@@ -2826,7 +2868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N110" authorId="0">
+    <comment ref="N110" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000049000000}">
       <text>
         <r>
           <rPr>
@@ -2838,7 +2880,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O111" authorId="0">
+    <comment ref="O111" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00004A000000}">
       <text>
         <r>
           <rPr>
@@ -2851,7 +2893,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P111" authorId="0">
+    <comment ref="P111" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00004B000000}">
       <text>
         <r>
           <rPr>
@@ -2864,7 +2906,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M114" authorId="0">
+    <comment ref="M114" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00004C000000}">
       <text>
         <r>
           <rPr>
@@ -2877,7 +2919,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M115" authorId="0">
+    <comment ref="M115" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00004D000000}">
       <text>
         <r>
           <rPr>
@@ -2890,7 +2932,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O115" authorId="0">
+    <comment ref="O115" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00004E000000}">
       <text>
         <r>
           <rPr>
@@ -2903,7 +2945,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N116" authorId="1">
+    <comment ref="N116" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-00004F000000}">
       <text>
         <r>
           <rPr>
@@ -2927,7 +2969,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J117" authorId="0">
+    <comment ref="J117" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000050000000}">
       <text>
         <r>
           <rPr>
@@ -2940,7 +2982,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N117" authorId="0">
+    <comment ref="N117" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000051000000}">
       <text>
         <r>
           <rPr>
@@ -2953,7 +2995,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O118" authorId="0">
+    <comment ref="O118" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000052000000}">
       <text>
         <r>
           <rPr>
@@ -2966,7 +3008,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P118" authorId="0">
+    <comment ref="P118" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000053000000}">
       <text>
         <r>
           <rPr>
@@ -2979,7 +3021,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J122" authorId="0">
+    <comment ref="J122" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000054000000}">
       <text>
         <r>
           <rPr>
@@ -2991,7 +3033,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O123" authorId="0">
+    <comment ref="O123" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000055000000}">
       <text>
         <r>
           <rPr>
@@ -3003,7 +3045,40 @@
         </r>
       </text>
     </comment>
-    <comment ref="J126" authorId="0">
+    <comment ref="J125" authorId="2" shapeId="0" xr:uid="{96A8580B-1A6C-4F42-8AB3-432F5A173E21}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>filter on catches based on species composition to infer habitat</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J126" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000056000000}">
       <text>
         <r>
           <rPr>
@@ -3015,7 +3090,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N126" authorId="0">
+    <comment ref="N126" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000057000000}">
       <text>
         <r>
           <rPr>
@@ -3027,7 +3102,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N127" authorId="0">
+    <comment ref="N127" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000058000000}">
       <text>
         <r>
           <rPr>
@@ -3040,7 +3115,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N131" authorId="0">
+    <comment ref="N131" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000059000000}">
       <text>
         <r>
           <rPr>
@@ -3053,7 +3128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N156" authorId="0">
+    <comment ref="N156" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00005A000000}">
       <text>
         <r>
           <rPr>
@@ -3065,7 +3140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O163" authorId="0">
+    <comment ref="O163" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00005B000000}">
       <text>
         <r>
           <rPr>
@@ -3078,7 +3153,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O164" authorId="0">
+    <comment ref="O164" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00005C000000}">
       <text>
         <r>
           <rPr>
@@ -3091,7 +3166,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O165" authorId="0">
+    <comment ref="O165" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00005D000000}">
       <text>
         <r>
           <rPr>
@@ -3104,7 +3179,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O167" authorId="0">
+    <comment ref="O167" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00005E000000}">
       <text>
         <r>
           <rPr>
@@ -3117,7 +3192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O169" authorId="0">
+    <comment ref="O169" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00005F000000}">
       <text>
         <r>
           <rPr>
@@ -3130,7 +3205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O170" authorId="0">
+    <comment ref="O170" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000060000000}">
       <text>
         <r>
           <rPr>
@@ -3143,7 +3218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O171" authorId="0">
+    <comment ref="O171" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000061000000}">
       <text>
         <r>
           <rPr>
@@ -3156,7 +3231,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O172" authorId="0">
+    <comment ref="O172" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000062000000}">
       <text>
         <r>
           <rPr>
@@ -3169,7 +3244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O173" authorId="0">
+    <comment ref="O173" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000063000000}">
       <text>
         <r>
           <rPr>
@@ -3182,7 +3257,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O174" authorId="0">
+    <comment ref="O174" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000064000000}">
       <text>
         <r>
           <rPr>
@@ -3195,7 +3270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O175" authorId="0">
+    <comment ref="O175" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000065000000}">
       <text>
         <r>
           <rPr>
@@ -3208,7 +3283,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O176" authorId="0">
+    <comment ref="O176" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000066000000}">
       <text>
         <r>
           <rPr>
@@ -3221,7 +3296,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O177" authorId="0">
+    <comment ref="O177" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000067000000}">
       <text>
         <r>
           <rPr>
@@ -3234,7 +3309,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O178" authorId="0">
+    <comment ref="O178" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000068000000}">
       <text>
         <r>
           <rPr>
@@ -3247,7 +3322,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O179" authorId="0">
+    <comment ref="O179" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000069000000}">
       <text>
         <r>
           <rPr>
@@ -3260,7 +3335,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L180" authorId="0">
+    <comment ref="L180" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00006A000000}">
       <text>
         <r>
           <rPr>
@@ -3272,7 +3347,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N183" authorId="0">
+    <comment ref="N183" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00006B000000}">
       <text>
         <r>
           <rPr>
@@ -3284,7 +3359,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O187" authorId="0">
+    <comment ref="O187" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00006C000000}">
       <text>
         <r>
           <rPr>
@@ -3297,7 +3372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M192" authorId="0">
+    <comment ref="M192" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00006D000000}">
       <text>
         <r>
           <rPr>
@@ -3310,7 +3385,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O192" authorId="0">
+    <comment ref="O192" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00006E000000}">
       <text>
         <r>
           <rPr>
@@ -3323,7 +3398,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N194" authorId="0">
+    <comment ref="N194" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00006F000000}">
       <text>
         <r>
           <rPr>
@@ -3335,7 +3410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O194" authorId="0">
+    <comment ref="O194" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000070000000}">
       <text>
         <r>
           <rPr>
@@ -3347,7 +3422,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N196" authorId="1">
+    <comment ref="N196" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000071000000}">
       <text>
         <r>
           <rPr>
@@ -3371,7 +3446,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N199" authorId="1">
+    <comment ref="N199" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000072000000}">
       <text>
         <r>
           <rPr>
@@ -3395,7 +3470,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M200" authorId="0">
+    <comment ref="M200" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000073000000}">
       <text>
         <r>
           <rPr>
@@ -3407,7 +3482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K204" authorId="0">
+    <comment ref="K204" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000074000000}">
       <text>
         <r>
           <rPr>
@@ -3420,7 +3495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N204" authorId="0">
+    <comment ref="N204" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000075000000}">
       <text>
         <r>
           <rPr>
@@ -3432,7 +3507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K207" authorId="0">
+    <comment ref="K207" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000076000000}">
       <text>
         <r>
           <rPr>
@@ -3444,7 +3519,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K208" authorId="0">
+    <comment ref="K208" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000077000000}">
       <text>
         <r>
           <rPr>
@@ -3456,7 +3531,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J212" authorId="1">
+    <comment ref="J212" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000078000000}">
       <text>
         <r>
           <rPr>
@@ -3480,7 +3555,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O214" authorId="0">
+    <comment ref="O214" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000079000000}">
       <text>
         <r>
           <rPr>
@@ -3492,7 +3567,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J217" authorId="0">
+    <comment ref="J217" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00007A000000}">
       <text>
         <r>
           <rPr>
@@ -3504,7 +3579,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N218" authorId="1">
+    <comment ref="N218" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-00007B000000}">
       <text>
         <r>
           <rPr>
@@ -3528,7 +3603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N219" authorId="0">
+    <comment ref="N219" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00007C000000}">
       <text>
         <r>
           <rPr>
@@ -3541,7 +3616,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F223" authorId="0">
+    <comment ref="F223" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-00007D000000}">
       <text>
         <r>
           <rPr>
@@ -3553,7 +3628,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J224" authorId="1">
+    <comment ref="J224" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-00007E000000}">
       <text>
         <r>
           <rPr>
@@ -3577,7 +3652,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N225" authorId="1">
+    <comment ref="N225" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-00007F000000}">
       <text>
         <r>
           <rPr>
@@ -3601,7 +3676,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J228" authorId="1">
+    <comment ref="J228" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000080000000}">
       <text>
         <r>
           <rPr>
@@ -3625,7 +3700,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N229" authorId="1">
+    <comment ref="N229" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000081000000}">
       <text>
         <r>
           <rPr>
@@ -3649,7 +3724,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J230" authorId="1">
+    <comment ref="J230" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0200-000082000000}">
       <text>
         <r>
           <rPr>
@@ -3673,7 +3748,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J231" authorId="0">
+    <comment ref="J231" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000083000000}">
       <text>
         <r>
           <rPr>
@@ -3685,7 +3760,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J232" authorId="0">
+    <comment ref="J232" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000084000000}">
       <text>
         <r>
           <rPr>
@@ -3697,7 +3772,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J233" authorId="0">
+    <comment ref="J233" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000085000000}">
       <text>
         <r>
           <rPr>
@@ -3709,7 +3784,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J234" authorId="0">
+    <comment ref="J234" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000086000000}">
       <text>
         <r>
           <rPr>
@@ -5447,8 +5522,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="16" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -5545,6 +5620,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -6016,6 +6104,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -6037,7 +6128,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 110"/>
+        <xdr:cNvPr id="2" name="AutoShape 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6093,7 +6190,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 110"/>
+        <xdr:cNvPr id="3" name="AutoShape 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6141,7 +6244,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 110"/>
+        <xdr:cNvPr id="4" name="AutoShape 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6197,7 +6306,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="AutoShape 110"/>
+        <xdr:cNvPr id="5" name="AutoShape 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6253,7 +6368,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="AutoShape 110"/>
+        <xdr:cNvPr id="6" name="AutoShape 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6301,7 +6422,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="AutoShape 110"/>
+        <xdr:cNvPr id="7" name="AutoShape 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6362,7 +6489,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1134" name="Rectangle 110" hidden="1"/>
+        <xdr:cNvPr id="1134" name="Rectangle 110" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-00006E040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6413,7 +6546,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 110"/>
+        <xdr:cNvPr id="2" name="AutoShape 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6469,7 +6608,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="AutoShape 110"/>
+        <xdr:cNvPr id="3" name="AutoShape 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6517,7 +6662,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="AutoShape 110"/>
+        <xdr:cNvPr id="4" name="AutoShape 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -6882,14 +7033,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V270"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="192" zoomScaleNormal="192" workbookViewId="0">
-      <pane xSplit="1" ySplit="8" topLeftCell="P9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="8" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
-      <selection pane="bottomRight" activeCell="A75" sqref="A75"/>
+      <selection pane="bottomRight" activeCell="U177" sqref="U177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6904,7 +7055,9 @@
     <col min="14" max="14" width="10.1640625" style="19" customWidth="1"/>
     <col min="15" max="18" width="8.83203125" style="19"/>
     <col min="19" max="19" width="11.6640625" style="19" customWidth="1"/>
-    <col min="20" max="22" width="8.83203125" style="19"/>
+    <col min="20" max="20" width="8.83203125" style="19"/>
+    <col min="21" max="21" width="14.33203125" style="19" customWidth="1"/>
+    <col min="22" max="22" width="29.83203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="14" x14ac:dyDescent="0.15">
@@ -18972,10 +19125,10 @@
         <v>523</v>
       </c>
       <c r="G177" s="21" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H177" s="21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I177" s="21">
         <v>0</v>
@@ -19014,7 +19167,7 @@
         <v>0</v>
       </c>
       <c r="U177" s="19" t="s">
-        <v>511</v>
+        <v>554</v>
       </c>
       <c r="V177" s="19" t="s">
         <v>511</v>
@@ -21081,6 +21234,9 @@
       <c r="V207" s="19" t="s">
         <v>511</v>
       </c>
+    </row>
+    <row r="208" spans="1:22" ht="14" x14ac:dyDescent="0.15">
+      <c r="A208" s="20"/>
     </row>
     <row r="269" spans="9:10" x14ac:dyDescent="0.15">
       <c r="I269" s="19" t="s">
@@ -21094,7 +21250,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V207">
+  <autoFilter ref="A1:V207" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState ref="A2:V207">
       <sortCondition ref="G1:G207"/>
     </sortState>
@@ -21112,7 +21268,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -21241,15 +21397,15 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AL234"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F219" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="163" zoomScaleNormal="163" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A285" sqref="A285"/>
+      <selection pane="bottomRight" activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -21400,7 +21556,7 @@
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
     </row>
-    <row r="3" spans="1:38" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:38" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>225</v>
       </c>
@@ -22828,7 +22984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:38" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:38" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="19" t="s">
         <v>466</v>
       </c>
@@ -24352,7 +24508,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="54" spans="1:38" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:38" ht="14" x14ac:dyDescent="0.15">
       <c r="A54" s="6" t="s">
         <v>271</v>
       </c>
@@ -25607,7 +25763,7 @@
       <c r="T75" s="9"/>
       <c r="U75" s="9"/>
     </row>
-    <row r="76" spans="1:21" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:21" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A76" s="6" t="s">
         <v>351</v>
       </c>
@@ -28320,7 +28476,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="125" spans="1:38" customFormat="1" ht="14" hidden="1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:38" customFormat="1" ht="14" x14ac:dyDescent="0.15">
       <c r="A125" s="6" t="s">
         <v>209</v>
       </c>
@@ -28346,10 +28502,10 @@
         <v>523</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J125" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K125" s="1">
         <v>0</v>
@@ -33070,7 +33226,7 @@
       <c r="AK212"/>
       <c r="AL212"/>
     </row>
-    <row r="213" spans="1:38" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A213" s="6" t="s">
         <v>237</v>
       </c>
@@ -33454,7 +33610,7 @@
       <c r="AK218" s="19"/>
       <c r="AL218" s="19"/>
     </row>
-    <row r="219" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:38" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A219" s="6" t="s">
         <v>30</v>
       </c>
@@ -33791,7 +33947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:38" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:38" customFormat="1" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A225" s="19" t="s">
         <v>30</v>
       </c>
@@ -34349,10 +34505,15 @@
       <c r="U234" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AL234">
+  <autoFilter ref="A1:AL234" xr:uid="{00000000-0009-0000-0000-000002000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="Yellowfin sole BSAI"/>
+        <filter val="Blue Crab Chesapeake Bay"/>
+        <filter val="Blue King Crab Pribilof Islands"/>
+        <filter val="Blue King Crab Saint Matthew"/>
+        <filter val="Blue Rockfish"/>
+        <filter val="bluefish - atlantic coast"/>
+        <filter val="Blueline Tilefish South Atlantic"/>
       </filters>
     </filterColumn>
     <sortState ref="A6:AL229">
@@ -34371,7 +34532,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>